<commit_message>
Most SAFM conventions added to Excel.
</commit_message>
<xml_diff>
--- a/ExcelExamples/Conventions.xlsx
+++ b/ExcelExamples/Conventions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Compounding" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>rate</t>
   </si>
@@ -35,16 +35,83 @@
   </si>
   <si>
     <t>QSA.RateConvert</t>
+  </si>
+  <si>
+    <t>QSA.DFFromRate</t>
+  </si>
+  <si>
+    <t>compounding</t>
+  </si>
+  <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>QSA.IsHoliday</t>
+  </si>
+  <si>
+    <t>date1</t>
+  </si>
+  <si>
+    <t>date2</t>
+  </si>
+  <si>
+    <t>convention</t>
+  </si>
+  <si>
+    <t>Act365</t>
+  </si>
+  <si>
+    <t>ActAct</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>calendar</t>
+  </si>
+  <si>
+    <t>ZaBusiness252</t>
+  </si>
+  <si>
+    <t>QSA.CreateBusiness252DayCount</t>
+  </si>
+  <si>
+    <t>Act360</t>
+  </si>
+  <si>
+    <t>30360EU</t>
+  </si>
+  <si>
+    <t>QSA.ApplyBusinessDayAdjustment</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>MF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000%"/>
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="ddd\ dd\-mmm\-yy"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,8 +127,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,6 +160,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -96,18 +182,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,15 +504,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C9"/>
+  <dimension ref="B3:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -444,7 +542,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -457,8 +555,79 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
-        <f ca="1">_xll.QSA.RateConvert(C4,C5,C6,C7)</f>
-        <v>0.10000000000000009</v>
+        <f>_xll.QSA.RateConvert(C4,C5,C6,C7)</f>
+        <v>9.5310179804324893E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <f>C4</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f>C5</f>
+        <v>Simple</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4">
+        <f>C7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <f>_xll.QSA.DFFromRate(C12,C13,C14)</f>
+        <v>0.90909090909090906</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <f>B9</f>
+        <v>9.5310179804324893E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="str">
+        <f>C6</f>
+        <v>Continuous</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4">
+        <f>C14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <f>_xll.QSA.DFFromRate(C19,C20,C21)</f>
+        <v>0.90909090909090906</v>
       </c>
     </row>
   </sheetData>
@@ -468,38 +637,247 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
+        <v>42813</v>
+      </c>
+      <c r="C7" s="9">
+        <f>_xll.QSA.IsHoliday(B7,$C$3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>42814</v>
+      </c>
+      <c r="C8" s="9">
+        <f>_xll.QSA.IsHoliday(B8,$C$3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>42815</v>
+      </c>
+      <c r="C9" s="9">
+        <f>_xll.QSA.IsHoliday(B9,$C$3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>42816</v>
+      </c>
+      <c r="C10" s="9">
+        <f>_xll.QSA.IsHoliday(B10,$C$3)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7">
+        <v>42430</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7">
+        <v>42795</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="10">
+        <f>_xll.QSA.GetYearFraction($C$3,$C$4,B7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="10">
+        <f>_xll.QSA.GetYearFraction($C$3,$C$4,B8)</f>
+        <v>1.0138888888888888</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="10">
+        <f>_xll.QSA.GetYearFraction($C$3,$C$4,B9)</f>
+        <v>0.9977094093869302</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="10">
+        <f>_xll.QSA.GetYearFraction($C$3,$C$4,B10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="str">
+        <f>B19</f>
+        <v>ZaBusiness252.07:44:44-1</v>
+      </c>
+      <c r="C11" s="10">
+        <f>_xll.QSA.GetYearFraction($C$3,$C$4,B11)</f>
+        <v>0.99206349206349209</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="str">
+        <f>_xll.QSA.CreateBusiness252DayCount(C16,C17)</f>
+        <v>ZaBusiness252.07:44:44-1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="7">
+        <v>42735</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="14">
+        <f ca="1">_xll.QSA.ApplyBusinessDayAdjustment(C4,C5,C6)</f>
+        <v>42734</v>
+      </c>
+      <c r="E8" s="13"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>